<commit_message>
guion tema 1 grado 08
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="95">
   <si>
     <t>FICHA</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Educación Básica Secundaria</t>
-  </si>
-  <si>
-    <t>MA</t>
   </si>
   <si>
     <t>Identifica la forma decimal de un número racional</t>
@@ -346,6 +343,12 @@
   </si>
   <si>
     <t>4° ESO</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Los números racionales e irracionales</t>
   </si>
 </sst>
 </file>
@@ -1862,7 +1865,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1897,21 +1900,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
         <v>91</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>92</v>
-      </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1925,19 +1928,19 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -1945,19 +1948,19 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -1965,19 +1968,19 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5">
         <v>6</v>
@@ -1985,19 +1988,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6">
         <v>11</v>
@@ -2005,19 +2008,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <v>13</v>
@@ -2026,19 +2029,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8">
         <v>16</v>
@@ -2047,19 +2050,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" t="s">
         <v>93</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
         <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
       </c>
       <c r="F9">
         <v>17</v>
@@ -2068,19 +2071,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
         <v>93</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <v>18</v>
@@ -2125,10 +2128,10 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2136,10 +2139,10 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -2147,10 +2150,10 @@
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>7</v>
@@ -2158,10 +2161,10 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -2169,10 +2172,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -2180,10 +2183,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>10</v>
@@ -2191,10 +2194,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -2202,10 +2205,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>14</v>
@@ -2213,10 +2216,10 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>15</v>
@@ -2224,10 +2227,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" s="17">
         <v>19</v>
@@ -2235,10 +2238,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>31</v>
       </c>
       <c r="C12" s="17">
         <v>20</v>
@@ -2292,10 +2295,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2303,10 +2306,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2314,10 +2317,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2325,10 +2328,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2336,10 +2339,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2347,10 +2350,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2358,10 +2361,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2369,10 +2372,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2380,10 +2383,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2391,10 +2394,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2402,10 +2405,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2413,10 +2416,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2424,10 +2427,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2435,10 +2438,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2446,10 +2449,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2457,10 +2460,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2468,10 +2471,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2479,10 +2482,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2490,10 +2493,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2501,10 +2504,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
         <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2584,13 +2587,13 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -2601,13 +2604,13 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
@@ -2618,13 +2621,13 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -2635,13 +2638,13 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -2652,15 +2655,15 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2669,15 +2672,15 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2686,167 +2689,167 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="49" t="s">
         <v>42</v>
-      </c>
-      <c r="E8" s="49" t="s">
-        <v>43</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H12" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="49" t="s">
-        <v>47</v>
-      </c>
       <c r="H14" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -2855,15 +2858,15 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
@@ -2872,159 +2875,159 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="54" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G25" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H25" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="D26" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -3033,15 +3036,15 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -3050,15 +3053,15 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -3067,15 +3070,15 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
       <c r="D29" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
@@ -3084,15 +3087,15 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
@@ -3101,89 +3104,89 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G32" s="49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G33" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="21"/>
       <c r="G34" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H34" s="69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D35" s="60"/>
       <c r="E35" s="61"/>
@@ -3194,15 +3197,15 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="24"/>
       <c r="D36" s="59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="24"/>
@@ -3211,36 +3214,36 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="26"/>
       <c r="D37" s="59" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E37" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
       <c r="H37" s="65" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="26"/>
       <c r="D38" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
@@ -3249,112 +3252,112 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="26"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
       <c r="F39" s="59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B40" s="23"/>
       <c r="C40" s="26"/>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H40" s="27"/>
       <c r="I40" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="26"/>
       <c r="D41" s="23"/>
       <c r="E41" s="24"/>
       <c r="F41" s="59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G41" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H41" s="65" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I41" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="26"/>
       <c r="D42" s="23"/>
       <c r="E42" s="24"/>
       <c r="F42" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="G42" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="H42" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="G42" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="H42" s="66" t="s">
-        <v>56</v>
-      </c>
       <c r="I42" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="26"/>
       <c r="D43" s="59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F43" s="23"/>
       <c r="G43" s="24"/>
       <c r="H43" s="67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I43" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
@@ -3365,13 +3368,13 @@
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -3382,13 +3385,13 @@
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B46" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29"/>
@@ -3399,13 +3402,13 @@
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
@@ -3416,15 +3419,15 @@
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B48" s="28"/>
       <c r="C48" s="31"/>
       <c r="D48" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="30"/>
@@ -3433,15 +3436,15 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B49" s="28"/>
       <c r="C49" s="31"/>
       <c r="D49" s="55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="29"/>
@@ -3450,15 +3453,15 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B50" s="28"/>
       <c r="C50" s="31"/>
       <c r="D50" s="57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F50" s="29"/>
       <c r="G50" s="29"/>
@@ -3467,15 +3470,15 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="31"/>
       <c r="D51" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="29"/>
@@ -3484,15 +3487,15 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B52" s="28"/>
       <c r="C52" s="31"/>
       <c r="D52" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
@@ -3501,15 +3504,15 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B53" s="28"/>
       <c r="C53" s="31"/>
       <c r="D53" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F53" s="29"/>
       <c r="G53" s="29"/>
@@ -3518,15 +3521,15 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" s="28"/>
       <c r="C54" s="29"/>
       <c r="D54" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" s="70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F54" s="29"/>
       <c r="G54" s="29"/>
@@ -3535,55 +3538,55 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55" s="28"/>
       <c r="C55" s="29"/>
       <c r="D55" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E55" s="56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
       <c r="H55" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I55" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
       <c r="D56" s="55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E56" s="56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="29"/>
       <c r="H56" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I56" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C57" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D57" s="36"/>
       <c r="E57" s="36"/>
@@ -3594,13 +3597,13 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D58" s="39"/>
       <c r="E58" s="36"/>
@@ -3611,15 +3614,15 @@
     </row>
     <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B59" s="35"/>
       <c r="C59" s="38"/>
       <c r="D59" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E59" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
@@ -3628,15 +3631,15 @@
     </row>
     <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B60" s="35"/>
       <c r="C60" s="38"/>
       <c r="D60" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E60" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F60" s="36"/>
       <c r="G60" s="36"/>
@@ -3645,15 +3648,15 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B61" s="35"/>
       <c r="C61" s="38"/>
       <c r="D61" s="71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E61" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
@@ -3662,53 +3665,53 @@
     </row>
     <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" s="35"/>
       <c r="C62" s="38"/>
       <c r="D62" s="71"/>
       <c r="E62" s="36"/>
       <c r="F62" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G62" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H62" s="37"/>
       <c r="I62" s="37"/>
     </row>
     <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="38"/>
       <c r="D63" s="71"/>
       <c r="E63" s="36"/>
       <c r="F63" s="71" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G63" s="72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H63" s="73" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I63" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B64" s="35"/>
       <c r="C64" s="38"/>
       <c r="D64" s="71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E64" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F64" s="36"/>
       <c r="G64" s="36"/>
@@ -3717,41 +3720,41 @@
     </row>
     <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" s="35"/>
       <c r="C65" s="38"/>
       <c r="D65" s="71"/>
       <c r="E65" s="37"/>
       <c r="F65" s="71" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G65" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H65" s="41"/>
       <c r="I65" s="37"/>
     </row>
     <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="38"/>
       <c r="D66" s="71"/>
       <c r="E66" s="36"/>
       <c r="F66" s="71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G66" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H66" s="40"/>
       <c r="I66" s="37"/>
     </row>
     <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B67" s="35"/>
       <c r="C67" s="36"/>
@@ -3759,66 +3762,66 @@
       <c r="E67" s="36"/>
       <c r="F67" s="36"/>
       <c r="G67" s="72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H67" s="41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I67" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B68" s="35"/>
       <c r="C68" s="36"/>
       <c r="D68" s="71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E68" s="72" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
       <c r="H68" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I68" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B69" s="74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C69" s="75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D69" s="45"/>
       <c r="E69" s="43"/>
       <c r="F69" s="43"/>
       <c r="G69" s="43"/>
       <c r="H69" s="86" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I69" s="44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B70" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D70" s="45"/>
       <c r="E70" s="43"/>
@@ -3826,18 +3829,18 @@
       <c r="G70" s="43"/>
       <c r="H70" s="44"/>
       <c r="I70" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D71" s="85"/>
       <c r="E71" s="43"/>
@@ -3845,7 +3848,7 @@
       <c r="G71" s="43"/>
       <c r="H71" s="44"/>
       <c r="I71" s="44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cambios recursos tema 1 grado octavo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="1"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="92">
   <si>
     <t>FICHA</t>
   </si>
@@ -141,12 +141,6 @@
     <t>Refuerza tu aprendizaje: Operaciones combinadas con números reale</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Las operaciones con números reales</t>
-  </si>
-  <si>
-    <t>MT_10_13</t>
-  </si>
-  <si>
     <t>sí</t>
   </si>
   <si>
@@ -229,9 +223,6 @@
   </si>
   <si>
     <t>Ejercitación y competencias</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Los números reales</t>
   </si>
   <si>
     <t>Refuerza tu aprendizaje: tipos de fracciones</t>
@@ -330,9 +321,6 @@
     </r>
   </si>
   <si>
-    <t>Competencias: Caracterización de los números reales</t>
-  </si>
-  <si>
     <t>Fin de tema</t>
   </si>
   <si>
@@ -342,13 +330,16 @@
     <t>Identifica la forma decimal de un número</t>
   </si>
   <si>
-    <t>4° ESO</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
     <t>Los números racionales e irracionales</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Operaciones con números reales</t>
+  </si>
+  <si>
+    <t>Competencias: Los números reales</t>
   </si>
 </sst>
 </file>
@@ -949,7 +940,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1109,6 +1100,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1864,8 +1858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1902,16 +1896,16 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1928,13 +1922,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -1948,13 +1942,13 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>26</v>
@@ -1968,13 +1962,13 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>32</v>
@@ -1988,13 +1982,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -2008,13 +2002,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -2029,13 +2023,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -2049,45 +2043,9 @@
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9">
-        <v>17</v>
-      </c>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>92</v>
-      </c>
-      <c r="B10" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10">
-        <v>18</v>
-      </c>
       <c r="G10" s="8"/>
     </row>
   </sheetData>
@@ -2103,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2128,7 +2086,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>30</v>
@@ -2139,7 +2097,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>30</v>
@@ -2161,7 +2119,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>30</v>
@@ -2172,7 +2130,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>30</v>
@@ -2183,7 +2141,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>30</v>
@@ -2194,7 +2152,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>30</v>
@@ -2205,7 +2163,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>30</v>
@@ -2216,7 +2174,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>30</v>
@@ -2226,24 +2184,46 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C13" s="17">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C14" s="17">
         <v>20</v>
       </c>
     </row>
@@ -2269,7 +2249,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2295,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -2309,7 +2289,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2320,7 +2300,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2331,7 +2311,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2339,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -2353,7 +2333,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2372,7 +2352,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -2383,7 +2363,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -2394,7 +2374,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -2408,7 +2388,7 @@
         <v>33</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2416,7 +2396,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -2430,7 +2410,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2438,7 +2418,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -2449,7 +2429,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
@@ -2463,29 +2443,29 @@
         <v>35</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>66</v>
+      <c r="B19" s="87" t="s">
+        <v>91</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2539,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2587,13 +2567,13 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="20"/>
       <c r="E2" s="20"/>
@@ -2604,13 +2584,13 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="20"/>
@@ -2621,13 +2601,13 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -2638,13 +2618,13 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -2655,15 +2635,15 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
       <c r="D6" s="50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
@@ -2672,15 +2652,15 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
       <c r="D7" s="50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
@@ -2689,20 +2669,20 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
       <c r="D8" s="50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="51" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>30</v>
@@ -2710,146 +2690,146 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="54" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="54" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="54" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H12" s="52" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G14" s="49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H14" s="22" t="s">
         <v>25</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="20"/>
       <c r="F15" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="G15" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="22" t="s">
-        <v>47</v>
-      </c>
       <c r="I15" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
       <c r="D16" s="53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="20"/>
@@ -2858,15 +2838,15 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="20"/>
@@ -2875,122 +2855,122 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G24" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>30</v>
@@ -2998,36 +2978,36 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G25" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H25" s="52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="D26" s="54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="20"/>
@@ -3036,15 +3016,15 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -3053,15 +3033,15 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -3070,15 +3050,15 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
       <c r="D29" s="54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
@@ -3087,15 +3067,15 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="54" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="20"/>
@@ -3104,51 +3084,51 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G32" s="49" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G33" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H33" s="68" t="s">
         <v>27</v>
@@ -3159,20 +3139,20 @@
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="21"/>
       <c r="G34" s="49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H34" s="69" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I34" s="18" t="s">
         <v>30</v>
@@ -3180,13 +3160,13 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B35" s="59" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D35" s="60"/>
       <c r="E35" s="61"/>
@@ -3197,15 +3177,15 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="24"/>
       <c r="D36" s="59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F36" s="24"/>
       <c r="G36" s="24"/>
@@ -3214,20 +3194,20 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="26"/>
       <c r="D37" s="59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E37" s="64" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
       <c r="H37" s="65" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I37" s="25" t="s">
         <v>30</v>
@@ -3235,15 +3215,15 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="26"/>
       <c r="D38" s="59" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
@@ -3252,34 +3232,34 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="26"/>
       <c r="D39" s="24"/>
       <c r="E39" s="24"/>
       <c r="F39" s="59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B40" s="23"/>
       <c r="C40" s="26"/>
       <c r="D40" s="24"/>
       <c r="E40" s="24"/>
       <c r="F40" s="59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H40" s="27"/>
       <c r="I40" s="25" t="s">
@@ -3288,62 +3268,62 @@
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="26"/>
       <c r="D41" s="23"/>
       <c r="E41" s="24"/>
       <c r="F41" s="59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G41" s="64" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H41" s="65" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I41" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="26"/>
       <c r="D42" s="23"/>
       <c r="E42" s="24"/>
       <c r="F42" s="59" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G42" s="64" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H42" s="66" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I42" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="26"/>
       <c r="D43" s="59" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E43" s="64" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F43" s="23"/>
       <c r="G43" s="24"/>
       <c r="H43" s="67" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I43" s="25" t="s">
         <v>30</v>
@@ -3351,13 +3331,13 @@
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B44" s="55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29"/>
@@ -3368,13 +3348,13 @@
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B45" s="55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29"/>
@@ -3385,13 +3365,13 @@
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B46" s="55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C46" s="70" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29"/>
@@ -3402,13 +3382,13 @@
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B47" s="55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
@@ -3419,15 +3399,15 @@
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B48" s="28"/>
       <c r="C48" s="31"/>
       <c r="D48" s="55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E48" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F48" s="28"/>
       <c r="G48" s="30"/>
@@ -3436,15 +3416,15 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B49" s="28"/>
       <c r="C49" s="31"/>
       <c r="D49" s="55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E49" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="29"/>
@@ -3453,15 +3433,15 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B50" s="28"/>
       <c r="C50" s="31"/>
       <c r="D50" s="57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F50" s="29"/>
       <c r="G50" s="29"/>
@@ -3470,15 +3450,15 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="31"/>
       <c r="D51" s="55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="29"/>
@@ -3487,15 +3467,15 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B52" s="28"/>
       <c r="C52" s="31"/>
       <c r="D52" s="55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
@@ -3504,15 +3484,15 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B53" s="28"/>
       <c r="C53" s="31"/>
       <c r="D53" s="55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E53" s="29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F53" s="29"/>
       <c r="G53" s="29"/>
@@ -3521,15 +3501,15 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B54" s="28"/>
       <c r="C54" s="29"/>
       <c r="D54" s="55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E54" s="70" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F54" s="29"/>
       <c r="G54" s="29"/>
@@ -3538,41 +3518,41 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B55" s="28"/>
       <c r="C55" s="29"/>
       <c r="D55" s="55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E55" s="56" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
       <c r="H55" s="33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I55" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
       <c r="D56" s="55" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E56" s="56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="29"/>
       <c r="H56" s="32" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I56" s="30" t="s">
         <v>30</v>
@@ -3580,13 +3560,13 @@
     </row>
     <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B57" s="71" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C57" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D57" s="36"/>
       <c r="E57" s="36"/>
@@ -3597,13 +3577,13 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B58" s="71" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C58" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D58" s="39"/>
       <c r="E58" s="36"/>
@@ -3614,15 +3594,15 @@
     </row>
     <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B59" s="35"/>
       <c r="C59" s="38"/>
       <c r="D59" s="71" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E59" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F59" s="36"/>
       <c r="G59" s="36"/>
@@ -3631,15 +3611,15 @@
     </row>
     <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B60" s="35"/>
       <c r="C60" s="38"/>
       <c r="D60" s="71" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E60" s="36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F60" s="36"/>
       <c r="G60" s="36"/>
@@ -3648,15 +3628,15 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B61" s="35"/>
       <c r="C61" s="38"/>
       <c r="D61" s="71" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E61" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
@@ -3665,37 +3645,37 @@
     </row>
     <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B62" s="35"/>
       <c r="C62" s="38"/>
       <c r="D62" s="71"/>
       <c r="E62" s="36"/>
       <c r="F62" s="71" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G62" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H62" s="37"/>
       <c r="I62" s="37"/>
     </row>
     <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="38"/>
       <c r="D63" s="71"/>
       <c r="E63" s="36"/>
       <c r="F63" s="71" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G63" s="72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H63" s="73" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I63" s="37" t="s">
         <v>30</v>
@@ -3703,15 +3683,15 @@
     </row>
     <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B64" s="35"/>
       <c r="C64" s="38"/>
       <c r="D64" s="71" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E64" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F64" s="36"/>
       <c r="G64" s="36"/>
@@ -3720,41 +3700,41 @@
     </row>
     <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B65" s="35"/>
       <c r="C65" s="38"/>
       <c r="D65" s="71"/>
       <c r="E65" s="37"/>
       <c r="F65" s="71" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G65" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H65" s="41"/>
       <c r="I65" s="37"/>
     </row>
     <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="38"/>
       <c r="D66" s="71"/>
       <c r="E66" s="36"/>
       <c r="F66" s="71" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G66" s="36" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H66" s="40"/>
       <c r="I66" s="37"/>
     </row>
     <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B67" s="35"/>
       <c r="C67" s="36"/>
@@ -3762,63 +3742,63 @@
       <c r="E67" s="36"/>
       <c r="F67" s="36"/>
       <c r="G67" s="72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H67" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I67" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B68" s="35"/>
       <c r="C68" s="36"/>
       <c r="D68" s="71" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E68" s="72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F68" s="36"/>
       <c r="G68" s="36"/>
       <c r="H68" s="41" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="I68" s="37" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B69" s="74" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C69" s="75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D69" s="45"/>
       <c r="E69" s="43"/>
       <c r="F69" s="43"/>
       <c r="G69" s="43"/>
       <c r="H69" s="86" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I69" s="44" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B70" s="45" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C70" s="42" t="s">
         <v>28</v>
@@ -3834,10 +3814,10 @@
     </row>
     <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C71" s="42" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
revisión esqueleto de guion
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CEN_3F_CDO_PC09\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PLANETA\Octavo\MA_08_01_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="11205" tabRatio="729" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="92">
   <si>
     <t>FICHA</t>
   </si>
@@ -220,9 +220,6 @@
   </si>
   <si>
     <t>Recuerda</t>
-  </si>
-  <si>
-    <t>Ejercitación y competencias</t>
   </si>
   <si>
     <t>Refuerza tu aprendizaje: tipos de fracciones</t>
@@ -340,6 +337,9 @@
   </si>
   <si>
     <t>Competencias: Los números reales</t>
+  </si>
+  <si>
+    <t>Competencias</t>
   </si>
 </sst>
 </file>
@@ -444,7 +444,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +499,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -940,7 +946,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1038,18 +1044,13 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1102,6 +1103,20 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="401">
@@ -1786,7 +1801,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,8 +1873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,16 +1911,16 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
         <v>86</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" t="s">
-        <v>87</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1922,13 +1937,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
         <v>88</v>
-      </c>
-      <c r="C3" t="s">
-        <v>89</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -1942,13 +1957,13 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>26</v>
@@ -1962,13 +1977,13 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
         <v>88</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>32</v>
@@ -1982,13 +1997,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
         <v>88</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -2002,13 +2017,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
         <v>88</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
       </c>
       <c r="D7" t="s">
         <v>34</v>
@@ -2023,13 +2038,13 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
         <v>88</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
       </c>
       <c r="D8" t="s">
         <v>35</v>
@@ -2086,7 +2101,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>30</v>
@@ -2097,7 +2112,7 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>30</v>
@@ -2119,7 +2134,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>30</v>
@@ -2130,7 +2145,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>30</v>
@@ -2141,7 +2156,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>30</v>
@@ -2152,7 +2167,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>30</v>
@@ -2163,7 +2178,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>30</v>
@@ -2184,8 +2199,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="87" t="s">
-        <v>90</v>
+      <c r="A11" s="84" t="s">
+        <v>89</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>30</v>
@@ -2195,8 +2210,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="87" t="s">
-        <v>91</v>
+      <c r="A12" s="84" t="s">
+        <v>90</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>30</v>
@@ -2275,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -2319,7 +2334,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -2352,7 +2367,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -2363,7 +2378,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -2374,7 +2389,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -2396,7 +2411,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -2418,7 +2433,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -2450,8 +2465,8 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="87" t="s">
-        <v>90</v>
+      <c r="B18" s="84" t="s">
+        <v>89</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>36</v>
@@ -2461,8 +2476,8 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="87" t="s">
-        <v>91</v>
+      <c r="B19" s="84" t="s">
+        <v>90</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>36</v>
@@ -2517,18 +2532,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="97" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="67.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
@@ -2567,7 +2582,7 @@
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>25</v>
@@ -2584,7 +2599,7 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>25</v>
@@ -2601,7 +2616,7 @@
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>25</v>
@@ -2618,7 +2633,7 @@
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>25</v>
@@ -2635,11 +2650,11 @@
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="54" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="20" t="s">
@@ -2652,11 +2667,11 @@
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="54" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="49" t="s">
@@ -2669,11 +2684,11 @@
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="54" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="49" t="s">
@@ -2682,7 +2697,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>30</v>
@@ -2690,7 +2705,7 @@
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
@@ -2707,7 +2722,7 @@
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
@@ -2724,7 +2739,7 @@
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
@@ -2741,7 +2756,7 @@
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
@@ -2762,7 +2777,7 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -2779,7 +2794,7 @@
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
@@ -2800,7 +2815,7 @@
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
@@ -2821,12 +2836,12 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
-      <c r="D16" s="53" t="s">
-        <v>72</v>
+      <c r="D16" s="91" t="s">
+        <v>71</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>37</v>
@@ -2838,12 +2853,12 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
       <c r="D17" s="53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>46</v>
@@ -2855,14 +2870,14 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>37</v>
@@ -2872,14 +2887,14 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>46</v>
@@ -2889,14 +2904,14 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>37</v>
@@ -2906,14 +2921,14 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>46</v>
@@ -2923,14 +2938,14 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>37</v>
@@ -2940,14 +2955,14 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
       <c r="F23" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>46</v>
@@ -2957,20 +2972,20 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G24" s="49" t="s">
         <v>40</v>
       </c>
       <c r="H24" s="51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I24" s="18" t="s">
         <v>30</v>
@@ -2978,14 +2993,14 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
       <c r="E25" s="20"/>
       <c r="F25" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25" s="49" t="s">
         <v>40</v>
@@ -2999,7 +3014,7 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -3016,7 +3031,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
@@ -3033,7 +3048,7 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
@@ -3050,7 +3065,7 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
@@ -3067,7 +3082,7 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
@@ -3084,7 +3099,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
@@ -3101,7 +3116,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
@@ -3118,7 +3133,7 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
@@ -3130,7 +3145,7 @@
       <c r="G33" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H33" s="68" t="s">
+      <c r="H33" s="65" t="s">
         <v>27</v>
       </c>
       <c r="I33" s="18" t="s">
@@ -3139,170 +3154,166 @@
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
-      <c r="D34" s="50" t="s">
+      <c r="D34" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="20"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="49" t="s">
+      <c r="E34" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="54"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="H34" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="I34" s="18" t="s">
+      <c r="F35" s="21"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="59" t="s">
-        <v>51</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="60"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="63"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="E36" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C36" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="58"/>
+      <c r="G36" s="58"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="60"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" s="23"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" s="64" t="s">
-        <v>40</v>
+      <c r="C37" s="24"/>
+      <c r="D37" s="86" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>37</v>
       </c>
       <c r="F37" s="24"/>
       <c r="G37" s="24"/>
-      <c r="H37" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="I37" s="25" t="s">
-        <v>30</v>
-      </c>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="26"/>
-      <c r="D38" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>37</v>
+      <c r="D38" s="86" t="s">
+        <v>74</v>
+      </c>
+      <c r="E38" s="61" t="s">
+        <v>40</v>
       </c>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
+      <c r="H38" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="G39" s="24" t="s">
+      <c r="D39" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="E39" s="24" t="s">
         <v>37</v>
       </c>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="23"/>
       <c r="C40" s="26"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="59" t="s">
+      <c r="D40" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="G40" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="H40" s="27"/>
-      <c r="I40" s="25" t="s">
-        <v>30</v>
-      </c>
+      <c r="E40" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="92"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="26"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="59" t="s">
+      <c r="D41" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="G41" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="H41" s="65" t="s">
-        <v>68</v>
-      </c>
+      <c r="E41" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="86"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="27"/>
       <c r="I41" s="25" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="26"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="59" t="s">
+      <c r="D42" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="G42" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="H42" s="66" t="s">
-        <v>53</v>
+      <c r="E42" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="86"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="62" t="s">
+        <v>67</v>
       </c>
       <c r="I42" s="25" t="s">
         <v>36</v>
@@ -3310,68 +3321,72 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="26"/>
-      <c r="D43" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" s="23"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="67" t="s">
-        <v>69</v>
+      <c r="D43" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="86"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="63" t="s">
+        <v>53</v>
       </c>
       <c r="I43" s="25" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="23"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
+      <c r="F44" s="86"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="90"/>
+      <c r="I44" s="25"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="30"/>
+        <v>70</v>
+      </c>
+      <c r="B45" s="23"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="F45" s="23"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="25" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="70" t="s">
-        <v>38</v>
+      <c r="A46" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="D46" s="29"/>
       <c r="E46" s="29"/>
@@ -3381,314 +3396,310 @@
       <c r="I46" s="30"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="55" t="s">
-        <v>78</v>
+      <c r="A47" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="87" t="s">
+        <v>77</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29"/>
       <c r="F47" s="28"/>
       <c r="G47" s="29"/>
-      <c r="H47" s="58"/>
+      <c r="H47" s="30"/>
       <c r="I47" s="30"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="28"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="E48" s="29" t="s">
+      <c r="A48" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F48" s="28"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="30"/>
-    </row>
-    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B49" s="28"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="28"/>
       <c r="G49" s="29"/>
-      <c r="H49" s="30"/>
+      <c r="H49" s="56"/>
       <c r="I49" s="30"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
-        <v>71</v>
+      <c r="A50" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B50" s="28"/>
       <c r="C50" s="31"/>
-      <c r="D50" s="57" t="s">
-        <v>56</v>
+      <c r="D50" s="87" t="s">
+        <v>54</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="30"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="33"/>
       <c r="I50" s="30"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
-        <v>71</v>
+      <c r="A51" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="31"/>
-      <c r="D51" s="55" t="s">
-        <v>79</v>
+      <c r="D51" s="87" t="s">
+        <v>55</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>37</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="29"/>
-      <c r="H51" s="33"/>
+      <c r="H51" s="30"/>
       <c r="I51" s="30"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
-        <v>71</v>
+      <c r="A52" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B52" s="28"/>
       <c r="C52" s="31"/>
-      <c r="D52" s="55" t="s">
-        <v>79</v>
+      <c r="D52" s="88" t="s">
+        <v>56</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F52" s="29"/>
       <c r="G52" s="29"/>
-      <c r="H52" s="33"/>
+      <c r="H52" s="30"/>
       <c r="I52" s="30"/>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="25" t="s">
-        <v>71</v>
+      <c r="A53" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B53" s="28"/>
       <c r="C53" s="31"/>
-      <c r="D53" s="55" t="s">
-        <v>79</v>
+      <c r="D53" s="87" t="s">
+        <v>78</v>
       </c>
       <c r="E53" s="29" t="s">
         <v>37</v>
       </c>
       <c r="F53" s="29"/>
       <c r="G53" s="29"/>
-      <c r="H53" s="34"/>
+      <c r="H53" s="33"/>
       <c r="I53" s="30"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="25" t="s">
-        <v>71</v>
+      <c r="A54" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B54" s="28"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="E54" s="70" t="s">
-        <v>38</v>
+      <c r="C54" s="31"/>
+      <c r="D54" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="F54" s="29"/>
       <c r="G54" s="29"/>
-      <c r="H54" s="30"/>
+      <c r="H54" s="33"/>
       <c r="I54" s="30"/>
     </row>
     <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
-        <v>71</v>
+      <c r="A55" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B55" s="28"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="E55" s="56" t="s">
-        <v>44</v>
+      <c r="C55" s="31"/>
+      <c r="D55" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
-      <c r="H55" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="I55" s="30" t="s">
-        <v>36</v>
-      </c>
+      <c r="H55" s="34"/>
+      <c r="I55" s="30"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
-        <v>71</v>
+      <c r="A56" s="30" t="s">
+        <v>70</v>
       </c>
       <c r="B56" s="28"/>
       <c r="C56" s="29"/>
-      <c r="D56" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="56" t="s">
-        <v>40</v>
+      <c r="D56" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="67" t="s">
+        <v>38</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="29"/>
-      <c r="H56" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="I56" s="30" t="s">
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="28"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" s="28"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="30"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B59" s="28"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="E59" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="I59" s="30" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B57" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="36" t="s">
+    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="39"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B59" s="35"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="E59" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-    </row>
-    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B60" s="35"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="E60" s="36" t="s">
-        <v>46</v>
-      </c>
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
       <c r="F60" s="36"/>
       <c r="G60" s="36"/>
       <c r="H60" s="37"/>
       <c r="I60" s="37"/>
     </row>
     <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B61" s="35"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="E61" s="36" t="s">
-        <v>37</v>
-      </c>
+      <c r="A61" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="39"/>
+      <c r="E61" s="36"/>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
       <c r="H61" s="37"/>
       <c r="I61" s="37"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="25" t="s">
-        <v>71</v>
+      <c r="A62" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="B62" s="35"/>
       <c r="C62" s="38"/>
-      <c r="D62" s="71"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="G62" s="36" t="s">
+      <c r="D62" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" s="36" t="s">
         <v>37</v>
       </c>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
       <c r="H62" s="37"/>
       <c r="I62" s="37"/>
     </row>
     <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="25" t="s">
-        <v>71</v>
+      <c r="A63" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="38"/>
-      <c r="D63" s="71"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="G63" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="H63" s="73" t="s">
-        <v>57</v>
-      </c>
-      <c r="I63" s="37" t="s">
-        <v>30</v>
-      </c>
+      <c r="D63" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="E63" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
     </row>
     <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="25" t="s">
-        <v>71</v>
+      <c r="A64" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="B64" s="35"/>
       <c r="C64" s="38"/>
-      <c r="D64" s="71" t="s">
-        <v>59</v>
+      <c r="D64" s="85" t="s">
+        <v>57</v>
       </c>
       <c r="E64" s="36" t="s">
         <v>37</v>
@@ -3699,277 +3710,351 @@
       <c r="I64" s="37"/>
     </row>
     <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="25" t="s">
-        <v>71</v>
+      <c r="A65" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="B65" s="35"/>
       <c r="C65" s="38"/>
-      <c r="D65" s="71"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="71" t="s">
-        <v>83</v>
+      <c r="D65" s="85"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="85" t="s">
+        <v>58</v>
       </c>
       <c r="G65" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="H65" s="41"/>
+      <c r="H65" s="37"/>
       <c r="I65" s="37"/>
     </row>
     <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="25" t="s">
-        <v>71</v>
+      <c r="A66" s="37" t="s">
+        <v>70</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="38"/>
-      <c r="D66" s="71"/>
+      <c r="D66" s="85"/>
       <c r="E66" s="36"/>
-      <c r="F66" s="71" t="s">
+      <c r="F66" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="G66" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="H66" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="I66" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67" s="35"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="E67" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="35"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="85"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="G68" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="41"/>
+      <c r="I68" s="37"/>
+    </row>
+    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="35"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="85"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="G66" s="36" t="s">
+      <c r="G69" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="H66" s="40"/>
-      <c r="I66" s="37"/>
-    </row>
-    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="72" t="s">
+      <c r="H69" s="40"/>
+      <c r="I69" s="37"/>
+    </row>
+    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="35"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="G70" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="H67" s="41" t="s">
+      <c r="H70" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="I67" s="37" t="s">
+      <c r="I70" s="37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="36"/>
-      <c r="D68" s="71" t="s">
+    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="35"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="E71" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="F71" s="36"/>
+      <c r="G71" s="69"/>
+      <c r="H71" s="41"/>
+      <c r="I71" s="37"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="35"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="85" t="s">
+        <v>83</v>
+      </c>
+      <c r="E72" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="I72" s="37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B73" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="45"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="I73" s="44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="E68" s="72" t="s">
-        <v>40</v>
-      </c>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="I68" s="37" t="s">
+      <c r="C74" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" s="45"/>
+      <c r="E74" s="43"/>
+      <c r="F74" s="43"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B69" s="74" t="s">
-        <v>63</v>
-      </c>
-      <c r="C69" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="D69" s="45"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="43"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="86" t="s">
-        <v>91</v>
-      </c>
-      <c r="I69" s="44" t="s">
+    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="D75" s="82"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="44" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="C70" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="D70" s="45"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="43"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="44"/>
-      <c r="I70" s="44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="C71" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D71" s="85"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="43"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="44"/>
-      <c r="I71" s="44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="76"/>
-      <c r="C72" s="77"/>
-      <c r="D72" s="78"/>
-      <c r="E72" s="79"/>
-      <c r="F72" s="78"/>
-      <c r="G72" s="79"/>
-      <c r="H72" s="5"/>
-    </row>
-    <row r="73" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
-      <c r="B73" s="76"/>
-      <c r="C73" s="77"/>
-      <c r="D73" s="78"/>
-      <c r="E73" s="79"/>
-      <c r="F73" s="78"/>
-      <c r="G73" s="79"/>
-      <c r="H73" s="80"/>
-    </row>
-    <row r="74" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
-      <c r="B74" s="76"/>
-      <c r="C74" s="77"/>
-      <c r="D74" s="78"/>
-      <c r="E74" s="79"/>
-      <c r="F74" s="79"/>
-      <c r="G74" s="79"/>
-      <c r="H74" s="5"/>
-    </row>
-    <row r="75" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="5"/>
-      <c r="B75" s="76"/>
-      <c r="C75" s="77"/>
-      <c r="D75" s="79"/>
-      <c r="E75" s="79"/>
-      <c r="F75" s="78"/>
-      <c r="G75" s="79"/>
-      <c r="H75" s="5"/>
     </row>
     <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
-      <c r="B76" s="76"/>
-      <c r="C76" s="77"/>
-      <c r="D76" s="79"/>
-      <c r="E76" s="79"/>
-      <c r="F76" s="78"/>
-      <c r="G76" s="79"/>
+      <c r="B76" s="73"/>
+      <c r="C76" s="74"/>
+      <c r="D76" s="75"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="75"/>
+      <c r="G76" s="76"/>
       <c r="H76" s="5"/>
     </row>
     <row r="77" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
-      <c r="B77" s="76"/>
-      <c r="C77" s="77"/>
-      <c r="D77" s="79"/>
-      <c r="E77" s="79"/>
-      <c r="F77" s="76"/>
-      <c r="G77" s="79"/>
-      <c r="H77" s="5"/>
+      <c r="B77" s="73"/>
+      <c r="C77" s="74"/>
+      <c r="D77" s="75"/>
+      <c r="E77" s="76"/>
+      <c r="F77" s="75"/>
+      <c r="G77" s="76"/>
+      <c r="H77" s="77"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
-      <c r="B78" s="76"/>
-      <c r="C78" s="77"/>
-      <c r="D78" s="79"/>
-      <c r="E78" s="79"/>
+      <c r="B78" s="73"/>
+      <c r="C78" s="74"/>
+      <c r="D78" s="75"/>
+      <c r="E78" s="76"/>
       <c r="F78" s="76"/>
-      <c r="G78" s="79"/>
+      <c r="G78" s="76"/>
       <c r="H78" s="5"/>
     </row>
     <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
-      <c r="B79" s="76"/>
-      <c r="C79" s="77"/>
-      <c r="D79" s="79"/>
-      <c r="E79" s="79"/>
-      <c r="F79" s="76"/>
-      <c r="G79" s="79"/>
-      <c r="H79" s="81"/>
+      <c r="B79" s="73"/>
+      <c r="C79" s="74"/>
+      <c r="D79" s="76"/>
+      <c r="E79" s="76"/>
+      <c r="F79" s="75"/>
+      <c r="G79" s="76"/>
+      <c r="H79" s="5"/>
     </row>
     <row r="80" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
-      <c r="B80" s="76"/>
-      <c r="C80" s="77"/>
+      <c r="B80" s="73"/>
+      <c r="C80" s="74"/>
       <c r="D80" s="76"/>
-      <c r="E80" s="79"/>
-      <c r="F80" s="79"/>
-      <c r="G80" s="79"/>
-      <c r="H80" s="81"/>
+      <c r="E80" s="76"/>
+      <c r="F80" s="75"/>
+      <c r="G80" s="76"/>
+      <c r="H80" s="5"/>
     </row>
     <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
-      <c r="B81" s="78"/>
-      <c r="C81" s="77"/>
+      <c r="B81" s="73"/>
+      <c r="C81" s="74"/>
       <c r="D81" s="76"/>
-      <c r="E81" s="79"/>
-      <c r="F81" s="79"/>
-      <c r="G81" s="79"/>
-      <c r="H81" s="81"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E81" s="76"/>
+      <c r="F81" s="73"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="B82" s="77"/>
-      <c r="C82" s="77"/>
-      <c r="D82" s="79"/>
-      <c r="E82" s="79"/>
-      <c r="F82" s="79"/>
-      <c r="G82" s="79"/>
+      <c r="B82" s="73"/>
+      <c r="C82" s="74"/>
+      <c r="D82" s="76"/>
+      <c r="E82" s="76"/>
+      <c r="F82" s="73"/>
+      <c r="G82" s="76"/>
       <c r="H82" s="5"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
-      <c r="B83" s="77"/>
-      <c r="C83" s="77"/>
-      <c r="D83" s="79"/>
-      <c r="E83" s="79"/>
-      <c r="F83" s="79"/>
-      <c r="G83" s="79"/>
-      <c r="H83" s="77"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="73"/>
+      <c r="C83" s="74"/>
+      <c r="D83" s="76"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="73"/>
+      <c r="G83" s="76"/>
+      <c r="H83" s="78"/>
+    </row>
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="B84" s="77"/>
-      <c r="C84" s="77"/>
-      <c r="D84" s="79"/>
-      <c r="E84" s="79"/>
-      <c r="F84" s="79"/>
-      <c r="G84" s="79"/>
-      <c r="H84" s="5"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="82"/>
-      <c r="B85" s="83"/>
-      <c r="C85" s="83"/>
-      <c r="D85" s="84"/>
-      <c r="E85" s="84"/>
-      <c r="F85" s="84"/>
-      <c r="G85" s="84"/>
-      <c r="H85" s="82"/>
+      <c r="B84" s="73"/>
+      <c r="C84" s="74"/>
+      <c r="D84" s="73"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="78"/>
+    </row>
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="5"/>
+      <c r="B85" s="75"/>
+      <c r="C85" s="74"/>
+      <c r="D85" s="73"/>
+      <c r="E85" s="76"/>
+      <c r="F85" s="76"/>
+      <c r="G85" s="76"/>
+      <c r="H85" s="78"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="74"/>
+      <c r="C86" s="74"/>
+      <c r="D86" s="76"/>
+      <c r="E86" s="76"/>
+      <c r="F86" s="76"/>
+      <c r="G86" s="76"/>
+      <c r="H86" s="5"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="74"/>
+      <c r="C87" s="74"/>
+      <c r="D87" s="76"/>
+      <c r="E87" s="76"/>
+      <c r="F87" s="76"/>
+      <c r="G87" s="76"/>
+      <c r="H87" s="74"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="5"/>
+      <c r="B88" s="74"/>
+      <c r="C88" s="74"/>
+      <c r="D88" s="76"/>
+      <c r="E88" s="76"/>
+      <c r="F88" s="76"/>
+      <c r="G88" s="76"/>
+      <c r="H88" s="5"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="79"/>
+      <c r="B89" s="80"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="81"/>
+      <c r="F89" s="81"/>
+      <c r="G89" s="81"/>
+      <c r="H89" s="79"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revisión esqueleto de guion Mat 8 tema 1
Aprobación del esqueleto
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="92">
   <si>
     <t>FICHA</t>
   </si>
@@ -228,9 +228,6 @@
     <t>La adición con números racionales</t>
   </si>
   <si>
-    <t>La multiplicación y división con números racionales</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: operaciones con números racionales</t>
   </si>
   <si>
@@ -307,6 +304,9 @@
   </si>
   <si>
     <t xml:space="preserve"> Consolidación </t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: números irracionales</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -988,7 +988,6 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1881,16 +1880,16 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" t="s">
-        <v>81</v>
       </c>
       <c r="E2" t="s">
         <v>30</v>
@@ -1907,13 +1906,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
         <v>82</v>
-      </c>
-      <c r="C3" t="s">
-        <v>83</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -1927,13 +1926,13 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
         <v>82</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>43</v>
@@ -1947,13 +1946,13 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>31</v>
@@ -1967,13 +1966,13 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
         <v>82</v>
-      </c>
-      <c r="C6" t="s">
-        <v>83</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
@@ -1987,13 +1986,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
         <v>82</v>
-      </c>
-      <c r="C7" t="s">
-        <v>83</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -2008,16 +2007,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" t="s">
-        <v>83</v>
-      </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -2069,124 +2068,124 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="72" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="71">
+      <c r="C2" s="70">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="72" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="71">
+      <c r="C3" s="70">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="72" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="70">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="72" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="70">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="70">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="70">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+    <row r="8" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="70">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="70" t="s">
+      <c r="B9" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="71">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="71">
+      <c r="C9" s="70">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="70" t="s">
+      <c r="B10" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="71">
+      <c r="C10" s="70">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
+    <row r="11" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="70">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="71">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="71">
+      <c r="C12" s="70">
         <v>18</v>
       </c>
     </row>
@@ -2256,10 +2255,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="70">
         <v>1</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="74" t="s">
         <v>61</v>
       </c>
       <c r="C2" t="s">
@@ -2267,10 +2266,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="71">
+      <c r="A3" s="70">
         <v>2</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="75" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2278,10 +2277,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="71">
+      <c r="A4" s="70">
         <v>3</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="75" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2289,10 +2288,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="71">
+      <c r="A5" s="70">
         <v>4</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="75" t="s">
         <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -2300,10 +2299,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="71">
+      <c r="A6" s="70">
         <v>5</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="74" t="s">
         <v>62</v>
       </c>
       <c r="C6" t="s">
@@ -2311,10 +2310,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="71">
+      <c r="A7" s="70">
         <v>6</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="75" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2322,10 +2321,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="71">
+      <c r="A8" s="70">
         <v>7</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="74" t="s">
         <v>26</v>
       </c>
       <c r="C8" t="s">
@@ -2333,10 +2332,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="71">
+      <c r="A9" s="70">
         <v>8</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="70" t="s">
         <v>63</v>
       </c>
       <c r="C9" t="s">
@@ -2344,10 +2343,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="71">
+      <c r="A10" s="70">
         <v>9</v>
       </c>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="74" t="s">
         <v>64</v>
       </c>
       <c r="C10" t="s">
@@ -2355,21 +2354,21 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="71">
+      <c r="A11" s="70">
         <v>10</v>
       </c>
-      <c r="B11" s="75" t="s">
-        <v>88</v>
+      <c r="B11" s="74" t="s">
+        <v>87</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="71">
+      <c r="A12" s="70">
         <v>11</v>
       </c>
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="70" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2377,21 +2376,21 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="71">
+      <c r="A13" s="70">
         <v>12</v>
       </c>
-      <c r="B13" s="71" t="s">
-        <v>66</v>
+      <c r="B13" s="70" t="s">
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="71">
+      <c r="A14" s="70">
         <v>13</v>
       </c>
-      <c r="B14" s="71" t="s">
+      <c r="B14" s="70" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -2399,21 +2398,21 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="71">
+      <c r="A15" s="70">
         <v>14</v>
       </c>
-      <c r="B15" s="71" t="s">
-        <v>67</v>
+      <c r="B15" s="70" t="s">
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="71">
+      <c r="A16" s="70">
         <v>15</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="74" t="s">
         <v>55</v>
       </c>
       <c r="C16" t="s">
@@ -2421,43 +2420,43 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="71">
+      <c r="A17" s="70">
         <v>16</v>
       </c>
-      <c r="B17" s="71" t="s">
-        <v>87</v>
+      <c r="B17" s="70" t="s">
+        <v>86</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="71">
+      <c r="A18" s="70">
         <v>17</v>
       </c>
-      <c r="B18" s="75" t="s">
-        <v>84</v>
+      <c r="B18" s="74" t="s">
+        <v>83</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="71">
+      <c r="A19" s="70">
         <v>18</v>
       </c>
-      <c r="B19" s="75" t="s">
-        <v>85</v>
+      <c r="B19" s="74" t="s">
+        <v>84</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="71">
+      <c r="A20" s="70">
         <v>19</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="73" t="s">
         <v>27</v>
       </c>
       <c r="C20" t="s">
@@ -2465,10 +2464,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="71">
+      <c r="A21" s="70">
         <v>20</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="73" t="s">
         <v>28</v>
       </c>
       <c r="C21" t="s">
@@ -2476,7 +2475,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="42"/>
+      <c r="B22" s="41"/>
       <c r="C22"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2504,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,7 +2512,7 @@
     <col min="1" max="1" width="49" customWidth="1"/>
     <col min="2" max="2" width="48.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="97" style="3" customWidth="1"/>
+    <col min="4" max="4" width="52.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="67.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
@@ -2552,9 +2551,9 @@
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="51" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="19" t="s">
@@ -2569,12 +2568,12 @@
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="42" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="19"/>
@@ -2586,9 +2585,9 @@
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="51" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -2603,9 +2602,9 @@
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="51" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -2620,11 +2619,13 @@
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="51" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="19" t="s">
@@ -2637,14 +2638,16 @@
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C7" s="18"/>
-      <c r="D7" s="52" t="s">
+      <c r="D7" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="42" t="s">
         <v>60</v>
       </c>
       <c r="F7" s="19"/>
@@ -2654,19 +2657,21 @@
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C8" s="18"/>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="42" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="76" t="s">
         <v>61</v>
       </c>
       <c r="I8" s="18" t="s">
@@ -2675,13 +2680,15 @@
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="51" t="s">
         <v>39</v>
       </c>
       <c r="G9" s="19" t="s">
@@ -2692,13 +2699,15 @@
     </row>
     <row r="10" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
-      <c r="F10" s="52" t="s">
+      <c r="F10" s="51" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="19" t="s">
@@ -2709,13 +2718,15 @@
     </row>
     <row r="11" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C11" s="18"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
-      <c r="F11" s="52" t="s">
+      <c r="F11" s="51" t="s">
         <v>40</v>
       </c>
       <c r="G11" s="19" t="s">
@@ -2726,19 +2737,21 @@
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="18"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="44" t="s">
+      <c r="H12" s="43" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="18" t="s">
@@ -2747,13 +2760,15 @@
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C13" s="18"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
-      <c r="F13" s="52" t="s">
+      <c r="F13" s="51" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="19" t="s">
@@ -2764,16 +2779,18 @@
     </row>
     <row r="14" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C14" s="18"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
-      <c r="F14" s="52" t="s">
+      <c r="F14" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="43" t="s">
+      <c r="G14" s="42" t="s">
         <v>42</v>
       </c>
       <c r="H14" s="21" t="s">
@@ -2785,16 +2802,18 @@
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="42" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="21" t="s">
@@ -2806,12 +2825,14 @@
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="77" t="s">
         <v>68</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="78" t="s">
-        <v>69</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>35</v>
@@ -2823,12 +2844,14 @@
     </row>
     <row r="17" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="78" t="s">
         <v>68</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="79" t="s">
-        <v>69</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>44</v>
@@ -2840,14 +2863,16 @@
     </row>
     <row r="18" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="52" t="s">
-        <v>70</v>
+      <c r="F18" s="51" t="s">
+        <v>69</v>
       </c>
       <c r="G18" s="19" t="s">
         <v>35</v>
@@ -2857,14 +2882,16 @@
     </row>
     <row r="19" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="52" t="s">
-        <v>70</v>
+      <c r="F19" s="51" t="s">
+        <v>69</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>44</v>
@@ -2874,14 +2901,16 @@
     </row>
     <row r="20" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
-      <c r="F20" s="52" t="s">
-        <v>70</v>
+      <c r="F20" s="51" t="s">
+        <v>69</v>
       </c>
       <c r="G20" s="19" t="s">
         <v>35</v>
@@ -2891,14 +2920,16 @@
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="52" t="s">
-        <v>70</v>
+      <c r="F21" s="51" t="s">
+        <v>69</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>44</v>
@@ -2908,14 +2939,16 @@
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
-      <c r="F22" s="52" t="s">
-        <v>71</v>
+      <c r="F22" s="51" t="s">
+        <v>70</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>35</v>
@@ -2925,14 +2958,16 @@
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="52" t="s">
-        <v>71</v>
+      <c r="F23" s="51" t="s">
+        <v>70</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>44</v>
@@ -2942,19 +2977,21 @@
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
-      <c r="F24" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="43" t="s">
+      <c r="F24" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H24" s="77" t="s">
+      <c r="H24" s="76" t="s">
         <v>62</v>
       </c>
       <c r="I24" s="18" t="s">
@@ -2963,19 +3000,21 @@
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
-      <c r="F25" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="43" t="s">
+      <c r="F25" s="51" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="44" t="s">
+      <c r="H25" s="43" t="s">
         <v>45</v>
       </c>
       <c r="I25" s="18" t="s">
@@ -2984,11 +3023,13 @@
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C26" s="18"/>
-      <c r="D26" s="52" t="s">
+      <c r="D26" s="51" t="s">
         <v>46</v>
       </c>
       <c r="E26" s="19" t="s">
@@ -3001,11 +3042,13 @@
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C27" s="18"/>
-      <c r="D27" s="52" t="s">
+      <c r="D27" s="51" t="s">
         <v>46</v>
       </c>
       <c r="E27" s="19" t="s">
@@ -3018,11 +3061,13 @@
     </row>
     <row r="28" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B28" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C28" s="18"/>
-      <c r="D28" s="52" t="s">
+      <c r="D28" s="51" t="s">
         <v>46</v>
       </c>
       <c r="E28" s="19" t="s">
@@ -3035,11 +3080,13 @@
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B29" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C29" s="18"/>
-      <c r="D29" s="52" t="s">
+      <c r="D29" s="51" t="s">
         <v>46</v>
       </c>
       <c r="E29" s="19" t="s">
@@ -3052,11 +3099,13 @@
     </row>
     <row r="30" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C30" s="18"/>
-      <c r="D30" s="52" t="s">
+      <c r="D30" s="51" t="s">
         <v>46</v>
       </c>
       <c r="E30" s="19" t="s">
@@ -3069,13 +3118,15 @@
     </row>
     <row r="31" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B31" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C31" s="18"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
-      <c r="F31" s="80" t="s">
+      <c r="F31" s="79" t="s">
         <v>47</v>
       </c>
       <c r="G31" s="19" t="s">
@@ -3086,16 +3137,18 @@
     </row>
     <row r="32" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B32" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
-      <c r="F32" s="80" t="s">
+      <c r="F32" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="G32" s="43" t="s">
+      <c r="G32" s="42" t="s">
         <v>60</v>
       </c>
       <c r="H32" s="18"/>
@@ -3103,19 +3156,21 @@
     </row>
     <row r="33" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B33" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C33" s="18"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
-      <c r="F33" s="80" t="s">
+      <c r="F33" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="G33" s="43" t="s">
+      <c r="G33" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="81" t="s">
+      <c r="H33" s="80" t="s">
         <v>26</v>
       </c>
       <c r="I33" s="18" t="s">
@@ -3124,36 +3179,40 @@
     </row>
     <row r="34" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B34" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C34" s="18"/>
-      <c r="D34" s="52" t="s">
+      <c r="D34" s="51" t="s">
         <v>48</v>
       </c>
       <c r="E34" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="52"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="81"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="80"/>
       <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="18"/>
+        <v>67</v>
+      </c>
+      <c r="B35" s="51" t="s">
+        <v>25</v>
+      </c>
       <c r="C35" s="18"/>
-      <c r="D35" s="80" t="s">
+      <c r="D35" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="43" t="s">
+      <c r="E35" s="42" t="s">
         <v>38</v>
       </c>
       <c r="F35" s="20"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="52" t="s">
+      <c r="G35" s="66"/>
+      <c r="H35" s="51" t="s">
         <v>63</v>
       </c>
       <c r="I35" s="18" t="s">
@@ -3162,29 +3221,31 @@
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="82" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="81" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>35</v>
       </c>
       <c r="D36" s="22"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="48"/>
-      <c r="I36" s="83"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="82"/>
     </row>
     <row r="37" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B37" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C37" s="23"/>
-      <c r="D37" s="84" t="s">
-        <v>72</v>
+      <c r="D37" s="83" t="s">
+        <v>71</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>35</v>
@@ -3196,19 +3257,21 @@
     </row>
     <row r="38" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B38" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C38" s="24"/>
-      <c r="D38" s="84" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" s="49" t="s">
+      <c r="D38" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="E38" s="48" t="s">
         <v>38</v>
       </c>
       <c r="F38" s="23"/>
       <c r="G38" s="23"/>
-      <c r="H38" s="51" t="s">
+      <c r="H38" s="50" t="s">
         <v>64</v>
       </c>
       <c r="I38" s="24" t="s">
@@ -3217,12 +3280,14 @@
     </row>
     <row r="39" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B39" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C39" s="24"/>
-      <c r="D39" s="84" t="s">
-        <v>73</v>
+      <c r="D39" s="83" t="s">
+        <v>72</v>
       </c>
       <c r="E39" s="23" t="s">
         <v>35</v>
@@ -3234,34 +3299,38 @@
     </row>
     <row r="40" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B40" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C40" s="24"/>
-      <c r="D40" s="84" t="s">
+      <c r="D40" s="83" t="s">
         <v>50</v>
       </c>
       <c r="E40" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="69"/>
+      <c r="F40" s="68"/>
       <c r="G40" s="23"/>
       <c r="H40" s="24"/>
       <c r="I40" s="24"/>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B41" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C41" s="24"/>
-      <c r="D41" s="84" t="s">
+      <c r="D41" s="83" t="s">
         <v>50</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="F41" s="84"/>
+      <c r="F41" s="83"/>
       <c r="G41" s="23"/>
       <c r="H41" s="25"/>
       <c r="I41" s="24" t="s">
@@ -3270,20 +3339,22 @@
     </row>
     <row r="42" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B42" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C42" s="24"/>
-      <c r="D42" s="84" t="s">
+      <c r="D42" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="84"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="51" t="s">
-        <v>65</v>
+      <c r="F42" s="83"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="50" t="s">
+        <v>87</v>
       </c>
       <c r="I42" s="24" t="s">
         <v>34</v>
@@ -3291,19 +3362,21 @@
     </row>
     <row r="43" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B43" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C43" s="24"/>
-      <c r="D43" s="84" t="s">
+      <c r="D43" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="49" t="s">
+      <c r="E43" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="F43" s="84"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="50" t="s">
+      <c r="F43" s="83"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="49" t="s">
         <v>51</v>
       </c>
       <c r="I43" s="24" t="s">
@@ -3312,37 +3385,41 @@
     </row>
     <row r="44" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B44" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C44" s="24"/>
-      <c r="D44" s="84" t="s">
-        <v>89</v>
+      <c r="D44" s="83" t="s">
+        <v>88</v>
       </c>
       <c r="E44" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F44" s="84"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="68"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="67"/>
       <c r="I44" s="24"/>
     </row>
     <row r="45" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="22"/>
+        <v>67</v>
+      </c>
+      <c r="B45" s="81" t="s">
+        <v>49</v>
+      </c>
       <c r="C45" s="24"/>
-      <c r="D45" s="82" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="49" t="s">
+      <c r="D45" s="81" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="48" t="s">
         <v>38</v>
       </c>
       <c r="F45" s="22"/>
       <c r="G45" s="23"/>
-      <c r="H45" s="51" t="s">
-        <v>66</v>
+      <c r="H45" s="50" t="s">
+        <v>65</v>
       </c>
       <c r="I45" s="24" t="s">
         <v>29</v>
@@ -3350,10 +3427,10 @@
     </row>
     <row r="46" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>35</v>
@@ -3367,10 +3444,10 @@
     </row>
     <row r="47" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>44</v>
@@ -3384,12 +3461,12 @@
     </row>
     <row r="48" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C48" s="85" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48" s="84" t="s">
         <v>36</v>
       </c>
       <c r="D48" s="27"/>
@@ -3401,10 +3478,10 @@
     </row>
     <row r="49" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>35</v>
@@ -3413,14 +3490,16 @@
       <c r="E49" s="27"/>
       <c r="F49" s="26"/>
       <c r="G49" s="27"/>
-      <c r="H49" s="46"/>
+      <c r="H49" s="45"/>
       <c r="I49" s="28"/>
     </row>
     <row r="50" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C50" s="28"/>
       <c r="D50" s="29" t="s">
         <v>52</v>
@@ -3435,9 +3514,11 @@
     </row>
     <row r="51" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B51" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C51" s="28"/>
       <c r="D51" s="29" t="s">
         <v>53</v>
@@ -3452,11 +3533,13 @@
     </row>
     <row r="52" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C52" s="28"/>
-      <c r="D52" s="46" t="s">
+      <c r="D52" s="45" t="s">
         <v>54</v>
       </c>
       <c r="E52" s="27" t="s">
@@ -3469,12 +3552,14 @@
     </row>
     <row r="53" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C53" s="28"/>
       <c r="D53" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E53" s="27" t="s">
         <v>35</v>
@@ -3486,12 +3571,14 @@
     </row>
     <row r="54" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C54" s="28"/>
       <c r="D54" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E54" s="27" t="s">
         <v>44</v>
@@ -3503,12 +3590,14 @@
     </row>
     <row r="55" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B55" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C55" s="28"/>
       <c r="D55" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E55" s="27" t="s">
         <v>35</v>
@@ -3520,14 +3609,16 @@
     </row>
     <row r="56" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B56" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C56" s="27"/>
       <c r="D56" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E56" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="E56" s="84" t="s">
         <v>36</v>
       </c>
       <c r="F56" s="27"/>
@@ -3537,20 +3628,22 @@
     </row>
     <row r="57" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B57" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C57" s="27"/>
       <c r="D57" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E57" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" s="44" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
       <c r="H57" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I57" s="28" t="s">
         <v>34</v>
@@ -3558,12 +3651,14 @@
     </row>
     <row r="58" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C58" s="27"/>
       <c r="D58" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E58" s="27" t="s">
         <v>35</v>
@@ -3575,462 +3670,488 @@
     </row>
     <row r="59" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="26"/>
+        <v>67</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>73</v>
+      </c>
       <c r="C59" s="27"/>
       <c r="D59" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E59" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E59" s="44" t="s">
         <v>38</v>
       </c>
       <c r="F59" s="27"/>
       <c r="G59" s="27"/>
       <c r="H59" s="29" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="I59" s="28" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="86" t="s">
+      <c r="A60" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B60" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C60" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+    </row>
+    <row r="61" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D61" s="34"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="32"/>
+      <c r="G61" s="32"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+    </row>
+    <row r="62" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="33"/>
+      <c r="D62" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E62" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="33"/>
+    </row>
+    <row r="63" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="33"/>
+      <c r="D63" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="33"/>
+    </row>
+    <row r="64" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="33"/>
+      <c r="D64" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="32"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+    </row>
+    <row r="65" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B65" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C65" s="33"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+    </row>
+    <row r="66" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C66" s="33"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G66" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="H66" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="I66" s="33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" s="33"/>
+      <c r="D67" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" s="32"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+    </row>
+    <row r="68" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" s="33"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="33"/>
+      <c r="F68" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="33" t="s">
+      <c r="G68" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="34"/>
-      <c r="I60" s="34"/>
-    </row>
-    <row r="61" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B61" s="86" t="s">
-        <v>77</v>
-      </c>
-      <c r="C61" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D61" s="35"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="34"/>
-      <c r="I61" s="34"/>
-    </row>
-    <row r="62" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B62" s="32"/>
-      <c r="C62" s="34"/>
-      <c r="D62" s="35" t="s">
+      <c r="H68" s="36"/>
+      <c r="I68" s="33"/>
+    </row>
+    <row r="69" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69" s="33"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="G69" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H69" s="35"/>
+      <c r="I69" s="33"/>
+    </row>
+    <row r="70" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="G70" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="H70" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="I70" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="32"/>
+      <c r="D71" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="E62" s="33" t="s">
+      <c r="E71" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="34"/>
-    </row>
-    <row r="63" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B63" s="32"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="35" t="s">
+      <c r="F71" s="32"/>
+      <c r="G71" s="52"/>
+      <c r="H71" s="36"/>
+      <c r="I71" s="33"/>
+    </row>
+    <row r="72" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" s="85" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="32"/>
+      <c r="D72" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="E63" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
-    </row>
-    <row r="64" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="32"/>
-      <c r="C64" s="34"/>
-      <c r="D64" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E64" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
-      <c r="H64" s="34"/>
-      <c r="I64" s="34"/>
-    </row>
-    <row r="65" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B65" s="32"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="G65" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H65" s="34"/>
-      <c r="I65" s="34"/>
-    </row>
-    <row r="66" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B66" s="32"/>
-      <c r="C66" s="34"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="33"/>
-      <c r="F66" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="G66" s="53" t="s">
+      <c r="E72" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="H66" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="I66" s="34" t="s">
+      <c r="F72" s="32"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="I72" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" s="32"/>
-      <c r="C67" s="34"/>
-      <c r="D67" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E67" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="34"/>
-      <c r="I67" s="34"/>
-    </row>
-    <row r="68" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B68" s="32"/>
-      <c r="C68" s="34"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="35" t="s">
+    <row r="73" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" s="39"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="I73" s="37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="G68" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H68" s="37"/>
-      <c r="I68" s="34"/>
-    </row>
-    <row r="69" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B69" s="32"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="86" t="s">
-        <v>58</v>
-      </c>
-      <c r="G69" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="H69" s="36"/>
-      <c r="I69" s="34"/>
-    </row>
-    <row r="70" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B70" s="32"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G70" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="H70" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="I70" s="34" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B71" s="32"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="F71" s="33"/>
-      <c r="G71" s="53"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="34"/>
-    </row>
-    <row r="72" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F72" s="33"/>
-      <c r="G72" s="33"/>
-      <c r="H72" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="I72" s="34" t="s">
+      <c r="C74" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="39"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B73" s="87" t="s">
-        <v>86</v>
-      </c>
-      <c r="C73" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="D73" s="40"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="66" t="s">
-        <v>85</v>
-      </c>
-      <c r="I73" s="38" t="s">
+    <row r="75" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B75" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" s="64"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="I75" s="37" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B74" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C74" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D74" s="40"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="39"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="38"/>
-      <c r="I74" s="38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="C75" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="D75" s="65"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="39"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="38"/>
-      <c r="I75" s="38" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="76" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="57"/>
-      <c r="B76" s="56"/>
-      <c r="C76" s="57"/>
-      <c r="D76" s="58"/>
-      <c r="E76" s="59"/>
-      <c r="F76" s="58"/>
-      <c r="G76" s="59"/>
-      <c r="H76" s="57"/>
-      <c r="I76" s="57"/>
+      <c r="A76" s="56"/>
+      <c r="B76" s="55"/>
+      <c r="C76" s="56"/>
+      <c r="D76" s="57"/>
+      <c r="E76" s="58"/>
+      <c r="F76" s="57"/>
+      <c r="G76" s="58"/>
+      <c r="H76" s="56"/>
+      <c r="I76" s="56"/>
     </row>
     <row r="77" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="57"/>
-      <c r="B77" s="56"/>
-      <c r="C77" s="57"/>
-      <c r="D77" s="58"/>
-      <c r="E77" s="59"/>
-      <c r="F77" s="58"/>
-      <c r="G77" s="59"/>
-      <c r="H77" s="60"/>
-      <c r="I77" s="57"/>
+      <c r="A77" s="56"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="56"/>
+      <c r="D77" s="57"/>
+      <c r="E77" s="58"/>
+      <c r="F77" s="57"/>
+      <c r="G77" s="58"/>
+      <c r="H77" s="59"/>
+      <c r="I77" s="56"/>
     </row>
     <row r="78" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="57"/>
-      <c r="B78" s="56"/>
-      <c r="C78" s="57"/>
-      <c r="D78" s="58"/>
-      <c r="E78" s="59"/>
-      <c r="F78" s="59"/>
-      <c r="G78" s="59"/>
-      <c r="H78" s="57"/>
-      <c r="I78" s="57"/>
+      <c r="A78" s="56"/>
+      <c r="B78" s="55"/>
+      <c r="C78" s="56"/>
+      <c r="D78" s="57"/>
+      <c r="E78" s="58"/>
+      <c r="F78" s="58"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="56"/>
+      <c r="I78" s="56"/>
     </row>
     <row r="79" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="57"/>
-      <c r="B79" s="56"/>
-      <c r="C79" s="57"/>
-      <c r="D79" s="59"/>
-      <c r="E79" s="59"/>
-      <c r="F79" s="58"/>
-      <c r="G79" s="59"/>
-      <c r="H79" s="57"/>
-      <c r="I79" s="57"/>
+      <c r="A79" s="56"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="56"/>
+      <c r="D79" s="58"/>
+      <c r="E79" s="58"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="58"/>
+      <c r="H79" s="56"/>
+      <c r="I79" s="56"/>
     </row>
     <row r="80" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="57"/>
-      <c r="B80" s="56"/>
-      <c r="C80" s="57"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="59"/>
-      <c r="F80" s="58"/>
-      <c r="G80" s="59"/>
-      <c r="H80" s="57"/>
-      <c r="I80" s="57"/>
+      <c r="A80" s="56"/>
+      <c r="B80" s="55"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="58"/>
+      <c r="E80" s="58"/>
+      <c r="F80" s="57"/>
+      <c r="G80" s="58"/>
+      <c r="H80" s="56"/>
+      <c r="I80" s="56"/>
     </row>
     <row r="81" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="57"/>
-      <c r="B81" s="56"/>
-      <c r="C81" s="57"/>
-      <c r="D81" s="59"/>
-      <c r="E81" s="59"/>
-      <c r="F81" s="56"/>
-      <c r="G81" s="59"/>
-      <c r="H81" s="57"/>
-      <c r="I81" s="57"/>
+      <c r="A81" s="56"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="56"/>
+      <c r="D81" s="58"/>
+      <c r="E81" s="58"/>
+      <c r="F81" s="55"/>
+      <c r="G81" s="58"/>
+      <c r="H81" s="56"/>
+      <c r="I81" s="56"/>
     </row>
     <row r="82" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
-      <c r="B82" s="56"/>
-      <c r="C82" s="57"/>
-      <c r="D82" s="59"/>
-      <c r="E82" s="59"/>
-      <c r="F82" s="56"/>
-      <c r="G82" s="59"/>
+      <c r="B82" s="55"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="58"/>
+      <c r="E82" s="58"/>
+      <c r="F82" s="55"/>
+      <c r="G82" s="58"/>
       <c r="H82" s="5"/>
     </row>
     <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
-      <c r="B83" s="56"/>
-      <c r="C83" s="57"/>
-      <c r="D83" s="59"/>
-      <c r="E83" s="59"/>
-      <c r="F83" s="56"/>
-      <c r="G83" s="59"/>
-      <c r="H83" s="61"/>
+      <c r="B83" s="55"/>
+      <c r="C83" s="56"/>
+      <c r="D83" s="58"/>
+      <c r="E83" s="58"/>
+      <c r="F83" s="55"/>
+      <c r="G83" s="58"/>
+      <c r="H83" s="60"/>
     </row>
     <row r="84" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
-      <c r="B84" s="56"/>
-      <c r="C84" s="57"/>
-      <c r="D84" s="56"/>
-      <c r="E84" s="59"/>
-      <c r="F84" s="59"/>
-      <c r="G84" s="59"/>
-      <c r="H84" s="61"/>
+      <c r="B84" s="55"/>
+      <c r="C84" s="56"/>
+      <c r="D84" s="55"/>
+      <c r="E84" s="58"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="58"/>
+      <c r="H84" s="60"/>
     </row>
     <row r="85" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
-      <c r="B85" s="58"/>
-      <c r="C85" s="57"/>
-      <c r="D85" s="56"/>
-      <c r="E85" s="59"/>
-      <c r="F85" s="59"/>
-      <c r="G85" s="59"/>
-      <c r="H85" s="61"/>
+      <c r="B85" s="57"/>
+      <c r="C85" s="56"/>
+      <c r="D85" s="55"/>
+      <c r="E85" s="58"/>
+      <c r="F85" s="58"/>
+      <c r="G85" s="58"/>
+      <c r="H85" s="60"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
-      <c r="B86" s="57"/>
-      <c r="C86" s="57"/>
-      <c r="D86" s="59"/>
-      <c r="E86" s="59"/>
-      <c r="F86" s="59"/>
-      <c r="G86" s="59"/>
+      <c r="B86" s="56"/>
+      <c r="C86" s="56"/>
+      <c r="D86" s="58"/>
+      <c r="E86" s="58"/>
+      <c r="F86" s="58"/>
+      <c r="G86" s="58"/>
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
-      <c r="B87" s="57"/>
-      <c r="C87" s="57"/>
-      <c r="D87" s="59"/>
-      <c r="E87" s="59"/>
-      <c r="F87" s="59"/>
-      <c r="G87" s="59"/>
-      <c r="H87" s="57"/>
+      <c r="B87" s="56"/>
+      <c r="C87" s="56"/>
+      <c r="D87" s="58"/>
+      <c r="E87" s="58"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="58"/>
+      <c r="H87" s="56"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
-      <c r="B88" s="57"/>
-      <c r="C88" s="57"/>
-      <c r="D88" s="59"/>
-      <c r="E88" s="59"/>
-      <c r="F88" s="59"/>
-      <c r="G88" s="59"/>
+      <c r="B88" s="56"/>
+      <c r="C88" s="56"/>
+      <c r="D88" s="58"/>
+      <c r="E88" s="58"/>
+      <c r="F88" s="58"/>
+      <c r="G88" s="58"/>
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="62"/>
-      <c r="B89" s="63"/>
-      <c r="C89" s="63"/>
-      <c r="D89" s="64"/>
-      <c r="E89" s="64"/>
-      <c r="F89" s="64"/>
-      <c r="G89" s="64"/>
-      <c r="H89" s="62"/>
+      <c r="A89" s="61"/>
+      <c r="B89" s="62"/>
+      <c r="C89" s="62"/>
+      <c r="D89" s="63"/>
+      <c r="E89" s="63"/>
+      <c r="F89" s="63"/>
+      <c r="G89" s="63"/>
+      <c r="H89" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MA0801: Ajustes de errores
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion01/esqueletoGuion_MA_08_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado08\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="11205" tabRatio="729" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15357" windowHeight="11203" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="86">
   <si>
     <t>FICHA</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Educación Básica Secundaria</t>
   </si>
   <si>
-    <t>Identifica la forma decimal de un número racional</t>
-  </si>
-  <si>
     <t>Los números racionales</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>Foto</t>
   </si>
   <si>
-    <t>La representación de los números racionales en la recta numérica</t>
-  </si>
-  <si>
     <t>El orden en los números racionales</t>
   </si>
   <si>
@@ -186,9 +180,6 @@
     <t>División de números racionales</t>
   </si>
   <si>
-    <t>Las operaciones con los números racionales</t>
-  </si>
-  <si>
     <t>Algunos números irracionales importantes</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>Multiplicación de números reales</t>
   </si>
   <si>
-    <t>Operaciones combinadas con números reales</t>
-  </si>
-  <si>
     <t>Recuerda</t>
   </si>
   <si>
@@ -258,9 +246,6 @@
     <t>Los números irracionales en la recta numérica</t>
   </si>
   <si>
-    <t>Conoce más sobre los números irracionales</t>
-  </si>
-  <si>
     <t>Los números reales</t>
   </si>
   <si>
@@ -291,9 +276,6 @@
     <t>Competencias</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Operaciones combinadas con números reales</t>
-  </si>
-  <si>
     <t>La multiplicación y la división con números racionales</t>
   </si>
   <si>
@@ -306,7 +288,7 @@
     <t xml:space="preserve"> Consolidación </t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: números irracionales</t>
+    <t>Refuerza tu aprendizaje: Operaciones combinadas con números reale</t>
   </si>
 </sst>
 </file>
@@ -1769,17 +1751,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -1787,7 +1769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
@@ -1803,7 +1785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
         <v>11</v>
       </c>
@@ -1811,7 +1793,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
@@ -1819,7 +1801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>12</v>
       </c>
@@ -1846,19 +1828,19 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
@@ -1878,21 +1860,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1904,132 +1886,132 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7">
         <v>13</v>
       </c>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>16</v>
       </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="8"/>
     </row>
   </sheetData>
@@ -2048,16 +2030,16 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
@@ -2068,144 +2050,144 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="71" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="70">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="71" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="70">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="71" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="70">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="71" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="71" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A5" s="40" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="70">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="70" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A6" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="70">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="70" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A7" s="15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B7" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="70">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="70" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A8" s="40" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="70">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="70" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A9" s="40" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B9" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="70">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="70" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A10" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="70">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="70" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A11" s="72" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B11" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="70">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="70" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="70" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A12" s="72" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="70">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="17">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="C14" s="17">
         <v>20</v>
@@ -2233,17 +2215,17 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -2254,234 +2236,234 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="70">
         <v>1</v>
       </c>
       <c r="B2" s="74" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="70">
         <v>2</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="70">
         <v>3</v>
       </c>
       <c r="B4" s="75" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A5" s="70">
         <v>4</v>
       </c>
       <c r="B5" s="75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A6" s="70">
         <v>5</v>
       </c>
       <c r="B6" s="74" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A7" s="70">
         <v>6</v>
       </c>
       <c r="B7" s="75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A8" s="70">
         <v>7</v>
       </c>
       <c r="B8" s="74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A9" s="70">
         <v>8</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A10" s="70">
         <v>9</v>
       </c>
       <c r="B10" s="74" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A11" s="70">
         <v>10</v>
       </c>
-      <c r="B11" s="74" t="s">
-        <v>87</v>
+      <c r="B11" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A12" s="70">
         <v>11</v>
       </c>
       <c r="B12" s="70" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A13" s="70">
         <v>12</v>
       </c>
       <c r="B13" s="70" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A14" s="70">
         <v>13</v>
       </c>
       <c r="B14" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A15" s="70">
         <v>14</v>
       </c>
       <c r="B15" s="70" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A16" s="70">
         <v>15</v>
       </c>
       <c r="B16" s="74" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A17" s="70">
         <v>16</v>
       </c>
       <c r="B17" s="70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A18" s="70">
         <v>17</v>
       </c>
       <c r="B18" s="74" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A19" s="70">
         <v>18</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A20" s="70">
         <v>19</v>
       </c>
       <c r="B20" s="73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A21" s="70">
         <v>20</v>
       </c>
       <c r="B21" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B22" s="41"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C23" s="4"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C28" s="6"/>
     </row>
   </sheetData>
@@ -2503,24 +2485,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView topLeftCell="E29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="52.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="67.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="65.5703125" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="52.86328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="67.1328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="65.59765625" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -2549,15 +2531,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
@@ -2566,15 +2548,15 @@
       <c r="H2" s="18"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
@@ -2583,15 +2565,15 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A4" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
@@ -2600,15 +2582,15 @@
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
     </row>
-    <row r="5" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A5" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
@@ -2617,617 +2599,617 @@
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
       <c r="H6" s="18"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A7" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A8" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="42" t="s">
         <v>37</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>38</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
       <c r="H8" s="76" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A9" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="18"/>
     </row>
-    <row r="10" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A11" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
       <c r="F11" s="51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
     </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A12" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
+      <c r="A13" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="51" t="s">
         <v>24</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>25</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
     </row>
-    <row r="14" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A14" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
       <c r="F14" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="42" t="s">
-        <v>42</v>
-      </c>
       <c r="H14" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
       <c r="F15" s="51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="77" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
     </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A17" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B17" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="78" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
     </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A18" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B18" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="51" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A19" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B19" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
       <c r="F19" s="51" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
     </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A20" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B20" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="51" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
     </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A21" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
       <c r="F21" s="51" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
     </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A22" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B22" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
       <c r="F22" s="51" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
     </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A23" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B23" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
       <c r="F23" s="51" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A24" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B24" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="19"/>
       <c r="E24" s="19"/>
       <c r="F24" s="51" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G24" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="76" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A25" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B25" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="51" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G25" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="43" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A26" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A27" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="18"/>
       <c r="D27" s="51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A28" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
     </row>
-    <row r="29" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A29" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A30" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A31" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="79" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A32" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="79" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G32" s="42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A33" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="79" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G33" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H33" s="80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A34" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F34" s="51"/>
       <c r="G34" s="42"/>
       <c r="H34" s="80"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A35" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="79" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="66"/>
       <c r="H35" s="51" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A36" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B36" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="22"/>
       <c r="E36" s="46"/>
@@ -3236,204 +3218,204 @@
       <c r="H36" s="47"/>
       <c r="I36" s="82"/>
     </row>
-    <row r="37" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A37" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B37" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="83" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
     </row>
-    <row r="38" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A38" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B38" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="83" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E38" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="23"/>
       <c r="G38" s="23"/>
       <c r="H38" s="50" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A39" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B39" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="83" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F39" s="23"/>
       <c r="G39" s="23"/>
       <c r="H39" s="24"/>
       <c r="I39" s="24"/>
     </row>
-    <row r="40" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A40" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B40" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="83" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F40" s="68"/>
       <c r="G40" s="23"/>
       <c r="H40" s="24"/>
       <c r="I40" s="24"/>
     </row>
-    <row r="41" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A41" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B41" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C41" s="24"/>
       <c r="D41" s="83" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F41" s="83"/>
       <c r="G41" s="23"/>
       <c r="H41" s="25"/>
       <c r="I41" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A42" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B42" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="83" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E42" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F42" s="83"/>
       <c r="G42" s="48"/>
-      <c r="H42" s="50" t="s">
-        <v>87</v>
+      <c r="H42" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="I42" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A43" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B43" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="24"/>
       <c r="D43" s="83" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E43" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F43" s="83"/>
       <c r="G43" s="48"/>
       <c r="H43" s="49" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="I43" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A44" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B44" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="83" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F44" s="83"/>
       <c r="G44" s="48"/>
       <c r="H44" s="67"/>
       <c r="I44" s="24"/>
     </row>
-    <row r="45" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A45" s="24" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B45" s="81" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="81" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E45" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F45" s="22"/>
       <c r="G45" s="23"/>
       <c r="H45" s="50" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A46" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
@@ -3442,15 +3424,15 @@
       <c r="H46" s="28"/>
       <c r="I46" s="28"/>
     </row>
-    <row r="47" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A47" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="27"/>
@@ -3459,15 +3441,15 @@
       <c r="H47" s="28"/>
       <c r="I47" s="28"/>
     </row>
-    <row r="48" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A48" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C48" s="84" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
@@ -3476,15 +3458,15 @@
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
     </row>
-    <row r="49" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A49" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49" s="27"/>
       <c r="E49" s="27"/>
@@ -3493,213 +3475,213 @@
       <c r="H49" s="45"/>
       <c r="I49" s="28"/>
     </row>
-    <row r="50" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A50" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C50" s="28"/>
       <c r="D50" s="29" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E50" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F50" s="26"/>
       <c r="G50" s="28"/>
       <c r="H50" s="30"/>
       <c r="I50" s="28"/>
     </row>
-    <row r="51" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A51" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C51" s="28"/>
       <c r="D51" s="29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E51" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F51" s="27"/>
       <c r="G51" s="27"/>
       <c r="H51" s="28"/>
       <c r="I51" s="28"/>
     </row>
-    <row r="52" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A52" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C52" s="28"/>
       <c r="D52" s="45" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F52" s="27"/>
       <c r="G52" s="27"/>
       <c r="H52" s="28"/>
       <c r="I52" s="28"/>
     </row>
-    <row r="53" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A53" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C53" s="28"/>
       <c r="D53" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E53" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F53" s="27"/>
       <c r="G53" s="27"/>
       <c r="H53" s="30"/>
       <c r="I53" s="28"/>
     </row>
-    <row r="54" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A54" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B54" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C54" s="28"/>
       <c r="D54" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E54" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F54" s="27"/>
       <c r="G54" s="27"/>
       <c r="H54" s="30"/>
       <c r="I54" s="28"/>
     </row>
-    <row r="55" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A55" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C55" s="28"/>
       <c r="D55" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F55" s="27"/>
       <c r="G55" s="27"/>
       <c r="H55" s="31"/>
       <c r="I55" s="28"/>
     </row>
-    <row r="56" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A56" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B56" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C56" s="27"/>
       <c r="D56" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E56" s="84" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F56" s="27"/>
       <c r="G56" s="27"/>
       <c r="H56" s="28"/>
       <c r="I56" s="28"/>
     </row>
-    <row r="57" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A57" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B57" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C57" s="27"/>
       <c r="D57" s="29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E57" s="44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F57" s="27"/>
       <c r="G57" s="27"/>
       <c r="H57" s="30" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="I57" s="28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A58" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C58" s="27"/>
       <c r="D58" s="29" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E58" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F58" s="27"/>
       <c r="G58" s="27"/>
       <c r="H58" s="30"/>
       <c r="I58" s="28"/>
     </row>
-    <row r="59" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A59" s="28" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C59" s="27"/>
       <c r="D59" s="29" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E59" s="44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F59" s="27"/>
       <c r="G59" s="27"/>
       <c r="H59" s="29" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="I59" s="28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A60" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B60" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D60" s="32"/>
       <c r="E60" s="32"/>
@@ -3708,15 +3690,15 @@
       <c r="H60" s="33"/>
       <c r="I60" s="33"/>
     </row>
-    <row r="61" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A61" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B61" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D61" s="34"/>
       <c r="E61" s="32"/>
@@ -3725,257 +3707,257 @@
       <c r="H61" s="33"/>
       <c r="I61" s="33"/>
     </row>
-    <row r="62" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A62" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B62" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C62" s="33"/>
       <c r="D62" s="34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E62" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F62" s="32"/>
       <c r="G62" s="32"/>
       <c r="H62" s="33"/>
       <c r="I62" s="33"/>
     </row>
-    <row r="63" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A63" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B63" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C63" s="33"/>
       <c r="D63" s="34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E63" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F63" s="32"/>
       <c r="G63" s="32"/>
       <c r="H63" s="33"/>
       <c r="I63" s="33"/>
     </row>
-    <row r="64" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A64" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B64" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C64" s="33"/>
       <c r="D64" s="34" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E64" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F64" s="32"/>
       <c r="G64" s="32"/>
       <c r="H64" s="33"/>
       <c r="I64" s="33"/>
     </row>
-    <row r="65" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A65" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B65" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C65" s="33"/>
       <c r="D65" s="34"/>
       <c r="E65" s="32"/>
       <c r="F65" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G65" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H65" s="33"/>
       <c r="I65" s="33"/>
     </row>
-    <row r="66" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A66" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B66" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C66" s="33"/>
       <c r="D66" s="34"/>
       <c r="E66" s="32"/>
       <c r="F66" s="34" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G66" s="52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H66" s="53" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I66" s="33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A67" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B67" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C67" s="33"/>
       <c r="D67" s="34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F67" s="32"/>
       <c r="G67" s="32"/>
       <c r="H67" s="33"/>
       <c r="I67" s="33"/>
     </row>
-    <row r="68" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A68" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B68" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C68" s="33"/>
       <c r="D68" s="34"/>
       <c r="E68" s="33"/>
       <c r="F68" s="34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G68" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H68" s="36"/>
       <c r="I68" s="33"/>
     </row>
-    <row r="69" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A69" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B69" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C69" s="33"/>
       <c r="D69" s="34"/>
       <c r="E69" s="32"/>
       <c r="F69" s="85" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G69" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H69" s="35"/>
       <c r="I69" s="33"/>
     </row>
-    <row r="70" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A70" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B70" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C70" s="32"/>
       <c r="D70" s="32"/>
       <c r="E70" s="32"/>
       <c r="F70" s="34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G70" s="52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H70" s="36" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="I70" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A71" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B71" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C71" s="32"/>
       <c r="D71" s="34" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E71" s="32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F71" s="32"/>
       <c r="G71" s="52"/>
       <c r="H71" s="36"/>
       <c r="I71" s="33"/>
     </row>
-    <row r="72" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A72" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B72" s="85" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C72" s="32"/>
       <c r="D72" s="34" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E72" s="52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F72" s="32"/>
       <c r="G72" s="32"/>
       <c r="H72" s="36" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I72" s="33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A73" s="37" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B73" s="86" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C73" s="54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D73" s="39"/>
       <c r="E73" s="38"/>
       <c r="F73" s="38"/>
       <c r="G73" s="38"/>
       <c r="H73" s="65" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I73" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A74" s="37" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C74" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D74" s="39"/>
       <c r="E74" s="38"/>
@@ -3983,31 +3965,31 @@
       <c r="G74" s="38"/>
       <c r="H74" s="37"/>
       <c r="I74" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A75" s="37" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C75" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D75" s="64"/>
       <c r="E75" s="38"/>
       <c r="F75" s="38"/>
       <c r="G75" s="38"/>
       <c r="H75" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="I75" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="I75" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A76" s="56"/>
       <c r="B76" s="55"/>
       <c r="C76" s="56"/>
@@ -4018,7 +4000,7 @@
       <c r="H76" s="56"/>
       <c r="I76" s="56"/>
     </row>
-    <row r="77" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A77" s="56"/>
       <c r="B77" s="55"/>
       <c r="C77" s="56"/>
@@ -4029,7 +4011,7 @@
       <c r="H77" s="59"/>
       <c r="I77" s="56"/>
     </row>
-    <row r="78" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A78" s="56"/>
       <c r="B78" s="55"/>
       <c r="C78" s="56"/>
@@ -4040,7 +4022,7 @@
       <c r="H78" s="56"/>
       <c r="I78" s="56"/>
     </row>
-    <row r="79" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A79" s="56"/>
       <c r="B79" s="55"/>
       <c r="C79" s="56"/>
@@ -4051,7 +4033,7 @@
       <c r="H79" s="56"/>
       <c r="I79" s="56"/>
     </row>
-    <row r="80" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A80" s="56"/>
       <c r="B80" s="55"/>
       <c r="C80" s="56"/>
@@ -4062,7 +4044,7 @@
       <c r="H80" s="56"/>
       <c r="I80" s="56"/>
     </row>
-    <row r="81" spans="1:9" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" s="2" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A81" s="56"/>
       <c r="B81" s="55"/>
       <c r="C81" s="56"/>
@@ -4073,7 +4055,7 @@
       <c r="H81" s="56"/>
       <c r="I81" s="56"/>
     </row>
-    <row r="82" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A82" s="5"/>
       <c r="B82" s="55"/>
       <c r="C82" s="56"/>
@@ -4083,7 +4065,7 @@
       <c r="G82" s="58"/>
       <c r="H82" s="5"/>
     </row>
-    <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A83" s="5"/>
       <c r="B83" s="55"/>
       <c r="C83" s="56"/>
@@ -4093,7 +4075,7 @@
       <c r="G83" s="58"/>
       <c r="H83" s="60"/>
     </row>
-    <row r="84" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A84" s="5"/>
       <c r="B84" s="55"/>
       <c r="C84" s="56"/>
@@ -4103,7 +4085,7 @@
       <c r="G84" s="58"/>
       <c r="H84" s="60"/>
     </row>
-    <row r="85" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A85" s="5"/>
       <c r="B85" s="57"/>
       <c r="C85" s="56"/>
@@ -4113,7 +4095,7 @@
       <c r="G85" s="58"/>
       <c r="H85" s="60"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="5"/>
       <c r="B86" s="56"/>
       <c r="C86" s="56"/>
@@ -4123,7 +4105,7 @@
       <c r="G86" s="58"/>
       <c r="H86" s="5"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="5"/>
       <c r="B87" s="56"/>
       <c r="C87" s="56"/>
@@ -4133,7 +4115,7 @@
       <c r="G87" s="58"/>
       <c r="H87" s="56"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="5"/>
       <c r="B88" s="56"/>
       <c r="C88" s="56"/>
@@ -4143,7 +4125,7 @@
       <c r="G88" s="58"/>
       <c r="H88" s="5"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="61"/>
       <c r="B89" s="62"/>
       <c r="C89" s="62"/>

</xml_diff>